<commit_message>
Added library attributions and release dates.
</commit_message>
<xml_diff>
--- a/RevA BOM.xlsx
+++ b/RevA BOM.xlsx
@@ -714,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H22" sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>